<commit_message>
Alteracao fPedido - QTD
</commit_message>
<xml_diff>
--- a/Documentacao/Acompanhamento e avaliação trabalho.xlsx
+++ b/Documentacao/Acompanhamento e avaliação trabalho.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IFES - COLATINA\Disciplinas\Delphi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ruan\Documents\SistemaVendasDelphi\Documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -582,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,7 +649,9 @@
         <v>1</v>
       </c>
       <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
+      <c r="E3" s="7">
+        <v>1</v>
+      </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -670,7 +672,9 @@
         <v>1</v>
       </c>
       <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
+      <c r="E4" s="7">
+        <v>1</v>
+      </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
@@ -691,7 +695,9 @@
         <v>2</v>
       </c>
       <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
+      <c r="E5" s="7">
+        <v>2</v>
+      </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -712,7 +718,9 @@
         <v>3</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
+      <c r="E6" s="7">
+        <v>3</v>
+      </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
@@ -733,7 +741,9 @@
         <v>2</v>
       </c>
       <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
+      <c r="E7" s="7">
+        <v>2</v>
+      </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -742,7 +752,7 @@
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
@@ -754,7 +764,9 @@
         <v>1</v>
       </c>
       <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="E8" s="7">
+        <v>1</v>
+      </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
@@ -775,7 +787,9 @@
         <v>1</v>
       </c>
       <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
+      <c r="E9" s="7">
+        <v>1</v>
+      </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
@@ -1006,7 +1020,9 @@
         <v>1</v>
       </c>
       <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
+      <c r="E20" s="7">
+        <v>1</v>
+      </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
@@ -1027,7 +1043,9 @@
         <v>1</v>
       </c>
       <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
+      <c r="E21" s="7">
+        <v>1</v>
+      </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
@@ -1073,7 +1091,7 @@
       </c>
       <c r="E23" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F23" s="8">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Tela de consultas add
</commit_message>
<xml_diff>
--- a/Documentacao/Acompanhamento e avaliação trabalho.xlsx
+++ b/Documentacao/Acompanhamento e avaliação trabalho.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="43">
   <si>
     <t>Cadastro de cliente (Nome, telefone, endereço, cnpj)</t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>Naiara</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>r</t>
   </si>
 </sst>
 </file>
@@ -266,7 +272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -299,6 +305,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -582,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,7 +819,9 @@
         <v>1</v>
       </c>
       <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
+      <c r="E10" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
@@ -831,7 +842,9 @@
         <v>1</v>
       </c>
       <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
+      <c r="E11" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
@@ -852,7 +865,9 @@
         <v>1</v>
       </c>
       <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
+      <c r="E12" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
@@ -873,7 +888,9 @@
         <v>1</v>
       </c>
       <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
+      <c r="E13" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
@@ -894,7 +911,9 @@
         <v>1</v>
       </c>
       <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
+      <c r="E14" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
@@ -936,7 +955,9 @@
         <v>1</v>
       </c>
       <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
+      <c r="E16" s="13" t="s">
+        <v>42</v>
+      </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
@@ -957,7 +978,9 @@
         <v>1</v>
       </c>
       <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
+      <c r="E17" s="13" t="s">
+        <v>41</v>
+      </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
@@ -978,7 +1001,9 @@
         <v>1</v>
       </c>
       <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
+      <c r="E18" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
@@ -999,7 +1024,9 @@
         <v>2</v>
       </c>
       <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
+      <c r="E19" s="7">
+        <v>2</v>
+      </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
@@ -1020,7 +1047,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="7"/>
-      <c r="E20" s="7">
+      <c r="E20" s="13">
         <v>1</v>
       </c>
       <c r="F20" s="7"/>
@@ -1066,7 +1093,9 @@
         <v>1</v>
       </c>
       <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
+      <c r="E22" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
@@ -1091,7 +1120,7 @@
       </c>
       <c r="E23" s="8">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F23" s="8">
         <f t="shared" si="1"/>
@@ -1214,7 +1243,7 @@
     <mergeCell ref="A28:B28"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1222,7 +1251,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A24" sqref="A24:XFD28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Consulta de Clientes sem venda por intervalo de data add
</commit_message>
<xml_diff>
--- a/Documentacao/Acompanhamento e avaliação trabalho.xlsx
+++ b/Documentacao/Acompanhamento e avaliação trabalho.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="43">
   <si>
     <t>Cadastro de cliente (Nome, telefone, endereço, cnpj)</t>
   </si>
@@ -300,14 +300,14 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -591,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,20 +603,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
     </row>
     <row r="2" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -819,8 +819,8 @@
         <v>1</v>
       </c>
       <c r="D10" s="7"/>
-      <c r="E10" s="7" t="s">
-        <v>42</v>
+      <c r="E10" s="7">
+        <v>1</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
@@ -842,7 +842,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="7"/>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="11" t="s">
         <v>42</v>
       </c>
       <c r="F11" s="7"/>
@@ -888,8 +888,8 @@
         <v>1</v>
       </c>
       <c r="D13" s="7"/>
-      <c r="E13" s="7" t="s">
-        <v>42</v>
+      <c r="E13" s="7">
+        <v>1</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
@@ -955,7 +955,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="7"/>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="11" t="s">
         <v>42</v>
       </c>
       <c r="F16" s="7"/>
@@ -978,7 +978,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="7"/>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="11" t="s">
         <v>41</v>
       </c>
       <c r="F17" s="7"/>
@@ -1047,7 +1047,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="7"/>
-      <c r="E20" s="13">
+      <c r="E20" s="11">
         <v>1</v>
       </c>
       <c r="F20" s="7"/>
@@ -1093,8 +1093,8 @@
         <v>1</v>
       </c>
       <c r="D22" s="7"/>
-      <c r="E22" s="7" t="s">
-        <v>41</v>
+      <c r="E22" s="7">
+        <v>1</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
@@ -1120,7 +1120,7 @@
       </c>
       <c r="E23" s="8">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F23" s="8">
         <f t="shared" si="1"/>
@@ -1192,10 +1192,10 @@
       <c r="L26" s="7"/>
     </row>
     <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="12"/>
+      <c r="B28" s="13"/>
       <c r="C28" s="8">
         <f>((C23*C25/100)+(C26*C23/100))/2</f>
         <v>23.75</v>
@@ -1263,20 +1263,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -1824,10 +1824,10 @@
       <c r="L26" s="7"/>
     </row>
     <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="12"/>
+      <c r="B28" s="13"/>
       <c r="C28" s="8">
         <f>((C23*C25/100)+(C26*C23/100))/2</f>
         <v>25</v>

</xml_diff>

<commit_message>
Consulta produtos mais vendidos implementado
</commit_message>
<xml_diff>
--- a/Documentacao/Acompanhamento e avaliação trabalho.xlsx
+++ b/Documentacao/Acompanhamento e avaliação trabalho.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="43">
   <si>
     <t>Cadastro de cliente (Nome, telefone, endereço, cnpj)</t>
   </si>
@@ -591,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,8 +842,8 @@
         <v>1</v>
       </c>
       <c r="D11" s="7"/>
-      <c r="E11" s="11" t="s">
-        <v>42</v>
+      <c r="E11" s="11">
+        <v>1</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
@@ -1120,7 +1120,7 @@
       </c>
       <c r="E23" s="8">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F23" s="8">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Add contorle de integridade do banco e erro solucionado em FPadrao
</commit_message>
<xml_diff>
--- a/Documentacao/Acompanhamento e avaliação trabalho.xlsx
+++ b/Documentacao/Acompanhamento e avaliação trabalho.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ruan\Documents\SistemaVendasDelphi\Documentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IFES - COLATINA\Disciplinas\Delphi\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
   <si>
     <t>Cadastro de cliente (Nome, telefone, endereço, cnpj)</t>
   </si>
@@ -148,12 +148,6 @@
   </si>
   <si>
     <t>Naiara</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>r</t>
   </si>
 </sst>
 </file>
@@ -272,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -299,9 +293,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -591,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,20 +594,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
     </row>
     <row r="2" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -658,9 +649,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="7"/>
-      <c r="E3" s="7">
-        <v>1</v>
-      </c>
+      <c r="E3" s="7"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -681,9 +670,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="7"/>
-      <c r="E4" s="7">
-        <v>1</v>
-      </c>
+      <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
@@ -704,9 +691,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="7"/>
-      <c r="E5" s="7">
-        <v>2</v>
-      </c>
+      <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -727,9 +712,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="E6" s="7">
-        <v>3</v>
-      </c>
+      <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
@@ -750,9 +733,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="7"/>
-      <c r="E7" s="7">
-        <v>2</v>
-      </c>
+      <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -761,7 +742,7 @@
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
     </row>
-    <row r="8" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
@@ -773,9 +754,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="7"/>
-      <c r="E8" s="7">
-        <v>1</v>
-      </c>
+      <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
@@ -796,9 +775,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="7"/>
-      <c r="E9" s="7">
-        <v>1</v>
-      </c>
+      <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
@@ -819,9 +796,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="7"/>
-      <c r="E10" s="7">
-        <v>1</v>
-      </c>
+      <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
@@ -842,9 +817,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="7"/>
-      <c r="E11" s="11">
-        <v>1</v>
-      </c>
+      <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
@@ -865,9 +838,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="7"/>
-      <c r="E12" s="7" t="s">
-        <v>42</v>
-      </c>
+      <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
@@ -888,9 +859,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="7"/>
-      <c r="E13" s="7">
-        <v>1</v>
-      </c>
+      <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
@@ -911,9 +880,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="7"/>
-      <c r="E14" s="7" t="s">
-        <v>41</v>
-      </c>
+      <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
@@ -955,9 +922,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="7"/>
-      <c r="E16" s="11" t="s">
-        <v>42</v>
-      </c>
+      <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
@@ -978,9 +943,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="7"/>
-      <c r="E17" s="11" t="s">
-        <v>41</v>
-      </c>
+      <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
@@ -1001,9 +964,7 @@
         <v>1</v>
       </c>
       <c r="D18" s="7"/>
-      <c r="E18" s="7" t="s">
-        <v>41</v>
-      </c>
+      <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
@@ -1024,9 +985,7 @@
         <v>2</v>
       </c>
       <c r="D19" s="7"/>
-      <c r="E19" s="7">
-        <v>2</v>
-      </c>
+      <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
@@ -1047,9 +1006,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="7"/>
-      <c r="E20" s="11">
-        <v>1</v>
-      </c>
+      <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
@@ -1070,9 +1027,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="7"/>
-      <c r="E21" s="7">
-        <v>1</v>
-      </c>
+      <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
@@ -1093,9 +1048,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="7"/>
-      <c r="E22" s="7">
-        <v>1</v>
-      </c>
+      <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
@@ -1120,7 +1073,7 @@
       </c>
       <c r="E23" s="8">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="F23" s="8">
         <f t="shared" si="1"/>
@@ -1192,10 +1145,10 @@
       <c r="L26" s="7"/>
     </row>
     <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="13"/>
+      <c r="B28" s="12"/>
       <c r="C28" s="8">
         <f>((C23*C25/100)+(C26*C23/100))/2</f>
         <v>23.75</v>
@@ -1243,7 +1196,7 @@
     <mergeCell ref="A28:B28"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1251,7 +1204,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A24" sqref="A24:XFD28"/>
     </sheetView>
   </sheetViews>
@@ -1263,20 +1216,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -1824,10 +1777,10 @@
       <c r="L26" s="7"/>
     </row>
     <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="13"/>
+      <c r="B28" s="12"/>
       <c r="C28" s="8">
         <f>((C23*C25/100)+(C26*C23/100))/2</f>
         <v>25</v>

</xml_diff>